<commit_message>
updated the ISA xls cheatsheet Added RTL files (Non-Functional)
</commit_message>
<xml_diff>
--- a/Doc/simple_cpu_isa.xlsx
+++ b/Doc/simple_cpu_isa.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="ISA_cheatsheet" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -385,7 +385,7 @@
   <dimension ref="A1:R25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="topLeft" activeCell="B37" activeCellId="0" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
incremental bug fixes, implemented control & status register, fixed the way RTL debug prints are done
</commit_message>
<xml_diff>
--- a/Doc/simple_cpu_isa.xlsx
+++ b/Doc/simple_cpu_isa.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="ISA_cheatsheet" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="69">
   <si>
     <t xml:space="preserve">BASE_OP_CODE</t>
   </si>
@@ -65,27 +65,27 @@
     <t xml:space="preserve">2K</t>
   </si>
   <si>
+    <t xml:space="preserve">USR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXT_OPS/USR_CONFIG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user configurable op_codes - 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JMP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADDR_MSB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">next byte has lsb for ADDR (I-type)</t>
+  </si>
+  <si>
     <t xml:space="preserve">CALL</t>
   </si>
   <si>
-    <t xml:space="preserve">ADDR_MSB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">next byte has lsb for ADDR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JMP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EXT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EXT_OPS/USR_CONFIG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">user configurable op_codes - 8</t>
-  </si>
-  <si>
     <t xml:space="preserve">ARITH</t>
   </si>
   <si>
@@ -140,7 +140,7 @@
     <t xml:space="preserve">reg3</t>
   </si>
   <si>
-    <t xml:space="preserve">DATA</t>
+    <t xml:space="preserve">DAT</t>
   </si>
   <si>
     <t xml:space="preserve">LD</t>
@@ -200,19 +200,34 @@
     <t xml:space="preserve">OVF</t>
   </si>
   <si>
-    <t xml:space="preserve">CONTROL_REG1</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> -</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16bit_mode</t>
+    <t xml:space="preserve">CR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONTROL_REG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SP_MSB10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SP_MSB9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SP_MSB8</t>
   </si>
   <si>
     <t xml:space="preserve">BCNZ</t>
   </si>
   <si>
     <t xml:space="preserve">BCZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STACK_POINTER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lower 8 bit of SP</t>
   </si>
 </sst>
 </file>
@@ -316,7 +331,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -335,6 +350,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -382,24 +401,26 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R25"/>
+  <dimension ref="A1:R29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B37" activeCellId="0" sqref="B37"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L34" activeCellId="0" sqref="L34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="6" style="0" width="8.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="33.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="13" style="0" width="8.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="14.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="16" style="0" width="8.72"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2955465587045"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.9271255060729"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.8259109311741"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.50607287449393"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.3400809716599"/>
+    <col collapsed="false" hidden="false" max="8" min="6" style="0" width="8.50607287449393"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.4777327935223"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="8.50607287449393"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="33.4574898785425"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="8.50607287449393"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="14.2591093117409"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="8.50607287449393"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -474,15 +495,15 @@
       <c r="F3" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2" t="s">
+      <c r="H3" s="5"/>
+      <c r="I3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
       <c r="L3" s="1" t="s">
         <v>9</v>
       </c>
@@ -499,7 +520,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="1"/>
       <c r="C4" s="4"/>
       <c r="D4" s="1" t="n">
@@ -511,20 +532,20 @@
       <c r="F4" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2" t="s">
+      <c r="H4" s="5"/>
+      <c r="I4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
       <c r="L4" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="1"/>
       <c r="C5" s="4"/>
       <c r="D5" s="1" t="n">
@@ -536,20 +557,20 @@
       <c r="F5" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
       <c r="L5" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="1"/>
       <c r="C6" s="4"/>
       <c r="D6" s="1" t="n">
@@ -561,17 +582,17 @@
       <c r="F6" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2" t="s">
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -590,7 +611,7 @@
       <c r="F7" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="6" t="s">
         <v>23</v>
       </c>
       <c r="H7" s="2" t="s">
@@ -622,7 +643,7 @@
       <c r="F8" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="6" t="s">
         <v>23</v>
       </c>
       <c r="H8" s="2" t="s">
@@ -665,7 +686,7 @@
       <c r="F9" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="G9" s="6" t="s">
         <v>23</v>
       </c>
       <c r="H9" s="2" t="s">
@@ -703,7 +724,7 @@
       <c r="F10" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="G10" s="6" t="s">
         <v>23</v>
       </c>
       <c r="H10" s="2" t="s">
@@ -741,7 +762,7 @@
       <c r="F11" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="G11" s="6" t="s">
         <v>23</v>
       </c>
       <c r="H11" s="2" t="s">
@@ -781,17 +802,17 @@
       <c r="F12" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="G12" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="H12" s="6"/>
-      <c r="I12" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
       <c r="L12" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="P12" s="0" t="n">
         <v>4</v>
@@ -817,17 +838,17 @@
       <c r="F13" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="H13" s="6"/>
-      <c r="I13" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
       <c r="L13" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="P13" s="0" t="n">
         <v>5</v>
@@ -837,10 +858,10 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
       <c r="P14" s="0" t="n">
         <v>6</v>
       </c>
@@ -849,10 +870,10 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
       <c r="P15" s="0" t="n">
         <v>7</v>
       </c>
@@ -921,16 +942,16 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D22" s="9" t="s">
+      <c r="D22" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="E22" s="9" t="s">
+      <c r="E22" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="F22" s="9" t="s">
+      <c r="F22" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="G22" s="9" t="s">
+      <c r="G22" s="10" t="s">
         <v>54</v>
       </c>
       <c r="H22" s="1" t="s">
@@ -948,10 +969,10 @@
     </row>
     <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D24" s="3" t="n">
         <v>7</v>
@@ -979,33 +1000,77 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D25" s="9" t="s">
+      <c r="D25" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="E25" s="10" t="s">
+      <c r="E25" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="F25" s="11" t="s">
+      <c r="F25" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="G25" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="H25" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="I25" s="10" t="s">
+      <c r="G25" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="J25" s="11" t="s">
+      <c r="H25" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="K25" s="11" t="s">
+      <c r="I25" s="11" t="s">
         <v>63</v>
       </c>
+      <c r="J25" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="K25" s="12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="D28" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="E28" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="F28" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="G28" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="H28" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="I28" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="J28" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K28" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D29" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8"/>
+      <c r="K29" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="31">
+  <mergeCells count="32">
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="C3:C6"/>
     <mergeCell ref="G3:H3"/>
@@ -1037,10 +1102,11 @@
     <mergeCell ref="J14:K14"/>
     <mergeCell ref="H15:I15"/>
     <mergeCell ref="J15:K15"/>
+    <mergeCell ref="D29:K29"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
Fixed a common mode error in cmodel/rtl on OR implementation. Added more tests
</commit_message>
<xml_diff>
--- a/Doc/simple_cpu_isa.xlsx
+++ b/Doc/simple_cpu_isa.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="70">
   <si>
     <t xml:space="preserve">BASE_OP_CODE</t>
   </si>
@@ -158,6 +158,15 @@
     <t xml:space="preserve">src_reg</t>
   </si>
   <si>
+    <t xml:space="preserve">SR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SP</t>
+  </si>
+  <si>
     <t xml:space="preserve">-</t>
   </si>
   <si>
@@ -179,9 +188,6 @@
     <t xml:space="preserve">PCSR (8 bit)</t>
   </si>
   <si>
-    <t xml:space="preserve">SR</t>
-  </si>
-  <si>
     <t xml:space="preserve">STATUS_REG</t>
   </si>
   <si>
@@ -219,9 +225,6 @@
   </si>
   <si>
     <t xml:space="preserve">BCZ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SP</t>
   </si>
   <si>
     <t xml:space="preserve">STACK_POINTER</t>
@@ -404,13 +407,13 @@
   <dimension ref="A1:R29"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L34" activeCellId="0" sqref="L34"/>
+      <selection pane="topLeft" activeCell="R15" activeCellId="0" sqref="R15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2955465587045"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.9271255060729"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.7894736842105"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.8259109311741"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.50607287449393"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.3400809716599"/>
@@ -856,6 +859,9 @@
       <c r="Q13" s="0" t="s">
         <v>45</v>
       </c>
+      <c r="R13" s="0" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H14" s="9"/>
@@ -866,7 +872,10 @@
         <v>6</v>
       </c>
       <c r="Q14" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
+      </c>
+      <c r="R14" s="0" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -878,43 +887,43 @@
         <v>7</v>
       </c>
       <c r="Q15" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="O17" s="0" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="0" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D21" s="3" t="n">
         <v>7</v>
@@ -943,36 +952,36 @@
     </row>
     <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D22" s="10" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="G22" s="10" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D24" s="3" t="n">
         <v>7</v>
@@ -1001,36 +1010,36 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D25" s="10" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="G25" s="12" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="H25" s="11" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="I25" s="11" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="J25" s="12" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="K25" s="12" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D28" s="3" t="n">
         <v>7</v>
@@ -1059,7 +1068,7 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D29" s="8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E29" s="8"/>
       <c r="F29" s="8"/>

</xml_diff>

<commit_message>
added support of array declaration in assembler. added support for alternate register access via reserved address 0-6. added support for indirect addressing
</commit_message>
<xml_diff>
--- a/Doc/simple_cpu_isa.xlsx
+++ b/Doc/simple_cpu_isa.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="71">
   <si>
     <t xml:space="preserve">BASE_OP_CODE</t>
   </si>
@@ -50,7 +50,7 @@
     <t xml:space="preserve">MISC OPS</t>
   </si>
   <si>
-    <t xml:space="preserve">NOP/RET/halt/rst/SET_BCZ/SET_BCNZ</t>
+    <t xml:space="preserve">NOP/RET/halt/SET_BCZ/SET_BCNZ/CLR_BC/SET_ADR_MODE/RST_ADR_MODE</t>
   </si>
   <si>
     <t xml:space="preserve">USER=&gt;</t>
@@ -210,6 +210,9 @@
   </si>
   <si>
     <t xml:space="preserve">CONTROL_REG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADR_MODE</t>
   </si>
   <si>
     <t xml:space="preserve">SP_MSB10</t>
@@ -406,8 +409,8 @@
   </sheetPr>
   <dimension ref="A1:R29"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R15" activeCellId="0" sqref="R15"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K34" activeCellId="0" sqref="K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -417,10 +420,11 @@
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.8259109311741"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.50607287449393"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.3400809716599"/>
-    <col collapsed="false" hidden="false" max="8" min="6" style="0" width="8.50607287449393"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.93522267206478"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="8.50607287449393"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="12.4777327935223"/>
     <col collapsed="false" hidden="false" max="11" min="10" style="0" width="8.50607287449393"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="33.4574898785425"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="62.6558704453441"/>
     <col collapsed="false" hidden="false" max="14" min="13" style="0" width="8.50607287449393"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="0" width="14.2591093117409"/>
     <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="8.50607287449393"/>
@@ -890,7 +894,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>49</v>
       </c>
@@ -1016,22 +1020,22 @@
         <v>48</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="G25" s="12" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H25" s="11" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I25" s="11" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J25" s="12" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="K25" s="12" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1039,7 +1043,7 @@
         <v>47</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D28" s="3" t="n">
         <v>7</v>
@@ -1068,7 +1072,7 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D29" s="8" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E29" s="8"/>
       <c r="F29" s="8"/>

</xml_diff>